<commit_message>
Fixed last bug, added max stack handle and class starting hour handle
</commit_message>
<xml_diff>
--- a/data/testdata/SSG_CLASSES.xlsx
+++ b/data/testdata/SSG_CLASSES.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27203"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_68FBE6C656FCFF9246D6A2A83B007F8FEA82F656" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF0644DE-6734-46F2-892F-E5635809A6BA}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_68FBE6C656FCFF9246D6A2A83B007F8FEA82F656" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48F64360-86CF-4623-82F7-364F09BC9EDB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -485,7 +485,7 @@
         <v>23</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6">

</xml_diff>